<commit_message>
Added a check for missing sequences
</commit_message>
<xml_diff>
--- a/PhasomeIt_data/phasomeit_out.xlsx
+++ b/PhasomeIt_data/phasomeit_out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u5501917/Documents/PhD/PhD/PhasomeIt_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80699266-6A94-E34C-B525-BD139A510F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709F9F04-91B4-7A4C-BD5D-F8E9137B5383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{480DD372-3942-D34A-8BED-516D6EDEA6F5}"/>
+    <workbookView xWindow="13680" yWindow="760" windowWidth="16560" windowHeight="18880" activeTab="3" xr2:uid="{480DD372-3942-D34A-8BED-516D6EDEA6F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Sheet 1" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5771" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5773" uniqueCount="1014">
   <si>
     <t>Name</t>
   </si>
@@ -3080,6 +3079,12 @@
   </si>
   <si>
     <t>Contig breaks in PilC2 make it impossible to resolve the full gene sequence or the repeat tract. Switch in expression between pilc1 and pilc2</t>
+  </si>
+  <si>
+    <t>N222.1.2_start</t>
+  </si>
+  <si>
+    <t>N222.1.2_stop</t>
   </si>
 </sst>
 </file>
@@ -3245,13 +3250,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>195618</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>157143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
+      <xdr:col>45</xdr:col>
       <xdr:colOff>276749</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>130628</xdr:rowOff>
@@ -8059,7 +8064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D96465A-A0A5-9846-835F-89D11FC7FBE7}">
   <dimension ref="A1:S305"/>
   <sheetViews>
-    <sheetView topLeftCell="A272" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A302" sqref="A302"/>
     </sheetView>
   </sheetViews>
@@ -12351,12 +12356,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30A245B-95BF-C943-9F83-1E9E02780E5F}">
-  <dimension ref="A1:AW95"/>
+  <dimension ref="A1:AY95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="88" zoomScaleNormal="112" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="X79" sqref="X79"/>
+      <selection pane="bottomLeft" activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12370,7 +12375,7 @@
     <col min="20" max="27" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>705</v>
       </c>
@@ -12489,37 +12494,43 @@
         <v>973</v>
       </c>
       <c r="AN1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AP1" t="s">
         <v>975</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>976</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>977</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>978</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>979</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>980</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>981</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>982</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>983</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>873</v>
       </c>
@@ -12637,8 +12648,14 @@
       <c r="AM2" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AN2">
+        <v>1872368</v>
+      </c>
+      <c r="AO2">
+        <v>1873705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>827</v>
       </c>
@@ -12756,8 +12773,14 @@
       <c r="AM3" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AN3">
+        <v>1867818</v>
+      </c>
+      <c r="AO3">
+        <v>1868321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4">
         <v>1</v>
@@ -12856,7 +12879,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5">
         <v>1</v>
@@ -12955,7 +12978,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6">
         <v>1</v>
@@ -13048,7 +13071,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7">
         <v>1</v>
@@ -13120,7 +13143,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8">
         <v>1</v>
@@ -13192,7 +13215,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9">
         <v>1</v>
@@ -13261,7 +13284,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>825</v>
       </c>
@@ -13376,8 +13399,14 @@
       <c r="AM10" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AN10">
+        <v>1855764</v>
+      </c>
+      <c r="AO10">
+        <v>1855246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>823</v>
       </c>
@@ -13486,8 +13515,14 @@
       <c r="AM11" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AN11">
+        <v>1836846</v>
+      </c>
+      <c r="AO11">
+        <v>1836562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12">
         <v>3</v>
@@ -13556,7 +13591,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>963</v>
       </c>
@@ -13657,7 +13692,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>901</v>
       </c>
@@ -13772,8 +13807,14 @@
       <c r="AM14" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AN14">
+        <v>1840400</v>
+      </c>
+      <c r="AO14">
+        <v>1837221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>741</v>
       </c>
@@ -13856,7 +13897,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>874</v>
       </c>
@@ -13971,8 +14012,14 @@
       <c r="AM16" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN16">
+        <v>1694881</v>
+      </c>
+      <c r="AO16">
+        <v>1693889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>875</v>
       </c>
@@ -14087,8 +14134,14 @@
       <c r="AM17" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN17">
+        <v>1664053</v>
+      </c>
+      <c r="AO17">
+        <v>1665177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>816</v>
       </c>
@@ -14203,8 +14256,14 @@
       <c r="AM18" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN18">
+        <v>1599318</v>
+      </c>
+      <c r="AO18">
+        <v>1598362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>816</v>
       </c>
@@ -14319,8 +14378,14 @@
       <c r="AM19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN19">
+        <v>1599318</v>
+      </c>
+      <c r="AO19">
+        <v>1598362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>813</v>
       </c>
@@ -14435,8 +14500,14 @@
       <c r="AM20" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN20">
+        <v>1562099</v>
+      </c>
+      <c r="AO20">
+        <v>1560240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>876</v>
       </c>
@@ -14551,8 +14622,14 @@
       <c r="AM21" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN21">
+        <v>1503201</v>
+      </c>
+      <c r="AO21">
+        <v>1503686</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>174</v>
       </c>
@@ -14641,7 +14718,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>809</v>
       </c>
@@ -14756,8 +14833,14 @@
       <c r="AM23" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN23">
+        <v>1455504</v>
+      </c>
+      <c r="AO23">
+        <v>1453858</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>188</v>
       </c>
@@ -14855,7 +14938,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>191</v>
       </c>
@@ -14938,7 +15021,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>190</v>
       </c>
@@ -15033,7 +15116,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>189</v>
       </c>
@@ -15119,7 +15202,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>877</v>
       </c>
@@ -15234,8 +15317,14 @@
       <c r="AM28" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN28">
+        <v>224113</v>
+      </c>
+      <c r="AO28">
+        <v>223754</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>803</v>
       </c>
@@ -15350,8 +15439,14 @@
       <c r="AM29" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN29">
+        <v>289712</v>
+      </c>
+      <c r="AO29">
+        <v>290612</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>878</v>
       </c>
@@ -15448,8 +15543,14 @@
       <c r="AM30" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN30">
+        <v>393693</v>
+      </c>
+      <c r="AO30">
+        <v>395366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>879</v>
       </c>
@@ -15564,8 +15665,14 @@
       <c r="AM31" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN31">
+        <v>485800</v>
+      </c>
+      <c r="AO31">
+        <v>483509</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>799</v>
       </c>
@@ -15671,8 +15778,14 @@
       <c r="AM32" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN32">
+        <v>623986</v>
+      </c>
+      <c r="AO32">
+        <v>623780</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>799</v>
       </c>
@@ -15751,8 +15864,14 @@
       <c r="AM33" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN33">
+        <v>623986</v>
+      </c>
+      <c r="AO33">
+        <v>623780</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>797</v>
       </c>
@@ -15861,8 +15980,14 @@
       <c r="AM34" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN34">
+        <v>654349</v>
+      </c>
+      <c r="AO34">
+        <v>653531</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>956</v>
       </c>
@@ -15951,7 +16076,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>794</v>
       </c>
@@ -16066,8 +16191,14 @@
       <c r="AM36" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN36">
+        <v>975236</v>
+      </c>
+      <c r="AO36">
+        <v>975791</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>282</v>
       </c>
@@ -16156,7 +16287,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>881</v>
       </c>
@@ -16271,8 +16402,14 @@
       <c r="AM38" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN38">
+        <v>1029612</v>
+      </c>
+      <c r="AO38">
+        <v>1028452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>880</v>
       </c>
@@ -16360,8 +16497,14 @@
       <c r="AM39" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN39">
+        <v>2003519</v>
+      </c>
+      <c r="AO39">
+        <v>2002530</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>880</v>
       </c>
@@ -16437,8 +16580,14 @@
       <c r="AM40" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN40">
+        <v>2003519</v>
+      </c>
+      <c r="AO40">
+        <v>2002530</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>952</v>
       </c>
@@ -16530,7 +16679,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>950</v>
       </c>
@@ -16645,8 +16794,14 @@
       <c r="AM42" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN42">
+        <v>1139948</v>
+      </c>
+      <c r="AO42">
+        <v>1138005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>788</v>
       </c>
@@ -16758,8 +16913,14 @@
       <c r="AM43" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN43">
+        <v>1212676</v>
+      </c>
+      <c r="AO43">
+        <v>1215285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>328</v>
       </c>
@@ -16848,7 +17009,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>785</v>
       </c>
@@ -16960,8 +17121,14 @@
       <c r="AM45" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN45">
+        <v>107533</v>
+      </c>
+      <c r="AO45">
+        <v>106701</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>783</v>
       </c>
@@ -17076,8 +17243,14 @@
       <c r="AM46" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN46">
+        <v>70171</v>
+      </c>
+      <c r="AO46">
+        <v>72039</v>
+      </c>
+    </row>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>781</v>
       </c>
@@ -17189,8 +17362,14 @@
       <c r="AM47" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN47">
+        <v>39736</v>
+      </c>
+      <c r="AO47">
+        <v>41019</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>882</v>
       </c>
@@ -17305,8 +17484,14 @@
       <c r="AM48" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN48">
+        <v>2140665</v>
+      </c>
+      <c r="AO48">
+        <v>2141711</v>
+      </c>
+    </row>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>778</v>
       </c>
@@ -17419,7 +17604,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>776</v>
       </c>
@@ -17528,8 +17713,14 @@
       <c r="AM50" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN50">
+        <v>2070341</v>
+      </c>
+      <c r="AO50">
+        <v>2068176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>883</v>
       </c>
@@ -17644,8 +17835,14 @@
       <c r="AM51" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN51">
+        <v>2056166</v>
+      </c>
+      <c r="AO51">
+        <v>2053053</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>772</v>
       </c>
@@ -17760,8 +17957,14 @@
       <c r="AM52" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN52">
+        <v>2011036</v>
+      </c>
+      <c r="AO52">
+        <v>2010032</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
       <c r="B53">
         <v>38</v>
@@ -17839,7 +18042,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>770</v>
       </c>
@@ -17951,8 +18154,14 @@
       <c r="AM54" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN54">
+        <v>2006234</v>
+      </c>
+      <c r="AO54">
+        <v>2005437</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>884</v>
       </c>
@@ -18067,8 +18276,14 @@
       <c r="AM55" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN55">
+        <v>1997654</v>
+      </c>
+      <c r="AO55">
+        <v>1996779</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>885</v>
       </c>
@@ -18180,8 +18395,14 @@
       <c r="AM56" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN56">
+        <v>1976062</v>
+      </c>
+      <c r="AO56">
+        <v>1975127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>766</v>
       </c>
@@ -18293,8 +18514,14 @@
       <c r="AM57" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN57">
+        <v>102353</v>
+      </c>
+      <c r="AO57">
+        <v>101173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>764</v>
       </c>
@@ -18404,7 +18631,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>485</v>
       </c>
@@ -18517,7 +18744,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>761</v>
       </c>
@@ -18632,8 +18859,14 @@
       <c r="AM60" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN60">
+        <v>803473</v>
+      </c>
+      <c r="AO60">
+        <v>804489</v>
+      </c>
+    </row>
+    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>759</v>
       </c>
@@ -18742,8 +18975,14 @@
       <c r="AM61" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN61">
+        <v>960475</v>
+      </c>
+      <c r="AO61">
+        <v>958934</v>
+      </c>
+    </row>
+    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
         <v>757</v>
       </c>
@@ -18858,8 +19097,14 @@
       <c r="AM62" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN62">
+        <v>1118857</v>
+      </c>
+      <c r="AO62">
+        <v>1120575</v>
+      </c>
+    </row>
+    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>755</v>
       </c>
@@ -18971,8 +19216,14 @@
       <c r="AM63" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN63">
+        <v>1163331</v>
+      </c>
+      <c r="AO63">
+        <v>1161085</v>
+      </c>
+    </row>
+    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>752</v>
       </c>
@@ -19087,8 +19338,14 @@
       <c r="AM64" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN64">
+        <v>1492696</v>
+      </c>
+      <c r="AO64">
+        <v>1491968</v>
+      </c>
+    </row>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>752</v>
       </c>
@@ -19182,8 +19439,14 @@
       <c r="AM65" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN65">
+        <v>1492696</v>
+      </c>
+      <c r="AO65">
+        <v>1491968</v>
+      </c>
+    </row>
+    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66">
         <v>51</v>
@@ -19264,7 +19527,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>750</v>
       </c>
@@ -19373,8 +19636,14 @@
       <c r="AM67" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN67">
+        <v>2097740</v>
+      </c>
+      <c r="AO67">
+        <v>2096661</v>
+      </c>
+    </row>
+    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>747</v>
       </c>
@@ -19474,8 +19743,14 @@
       <c r="AM68" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN68">
+        <v>1861502</v>
+      </c>
+      <c r="AO68">
+        <v>1861831</v>
+      </c>
+    </row>
+    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>759</v>
       </c>
@@ -19563,8 +19838,14 @@
       <c r="AM69" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN69">
+        <v>960475</v>
+      </c>
+      <c r="AO69">
+        <v>958934</v>
+      </c>
+    </row>
+    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>901</v>
       </c>
@@ -19652,8 +19933,14 @@
       <c r="AM70" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN70">
+        <v>1840400</v>
+      </c>
+      <c r="AO70">
+        <v>1837221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>901</v>
       </c>
@@ -19741,8 +20028,14 @@
       <c r="AM71" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN71">
+        <v>1840400</v>
+      </c>
+      <c r="AO71">
+        <v>1837221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>739</v>
       </c>
@@ -19845,8 +20138,14 @@
       <c r="AM72" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN72">
+        <v>1420853</v>
+      </c>
+      <c r="AO72">
+        <v>1419969</v>
+      </c>
+    </row>
+    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>737</v>
       </c>
@@ -19961,8 +20260,14 @@
       <c r="AM73" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN73">
+        <v>2073671</v>
+      </c>
+      <c r="AO73">
+        <v>2072325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>734</v>
       </c>
@@ -20077,8 +20382,14 @@
       <c r="AM74" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN74">
+        <v>1453733</v>
+      </c>
+      <c r="AO74">
+        <v>1452375</v>
+      </c>
+    </row>
+    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
         <v>732</v>
       </c>
@@ -20190,8 +20501,14 @@
       <c r="AM75" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN75">
+        <v>52203</v>
+      </c>
+      <c r="AO75">
+        <v>48988</v>
+      </c>
+    </row>
+    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>730</v>
       </c>
@@ -20306,8 +20623,14 @@
       <c r="AM76" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN76">
+        <v>1292015</v>
+      </c>
+      <c r="AO76">
+        <v>1291327</v>
+      </c>
+    </row>
+    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>728</v>
       </c>
@@ -20422,8 +20745,14 @@
       <c r="AM77" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN77">
+        <v>488885</v>
+      </c>
+      <c r="AO77">
+        <v>489601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>724</v>
       </c>
@@ -20538,8 +20867,14 @@
       <c r="AM78" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN78">
+        <v>972454</v>
+      </c>
+      <c r="AO78">
+        <v>973404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>722</v>
       </c>
@@ -20654,8 +20989,14 @@
       <c r="AM79" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN79">
+        <v>802559</v>
+      </c>
+      <c r="AO79">
+        <v>803152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
         <v>899</v>
       </c>

</xml_diff>